<commit_message>
added the capstone schedule
</commit_message>
<xml_diff>
--- a/CapstoneTimeScehdule.xlsx
+++ b/CapstoneTimeScehdule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Desktop\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,74 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Ended</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>9:00am
+11:00am</t>
+  </si>
+  <si>
+    <t>11:00am
+12:00am</t>
+  </si>
+  <si>
+    <t>4:00pm</t>
+  </si>
+  <si>
+    <t>9:00pm</t>
+  </si>
+  <si>
+    <t>9:00am
+11:00am
+5:30pm</t>
+  </si>
+  <si>
+    <t>11:00am
+12:00am
+8:00pm</t>
+  </si>
+  <si>
+    <t>•Created porject as well as set up my actual application | Research Native Script</t>
+  </si>
+  <si>
+    <t>•Researched Native Script
+•Started creating navigation
+•Finished navigating between multiple pages.| Created a simple user input section for testing</t>
+  </si>
+  <si>
+    <t>•Set up Firebase DB. | Added Firebase to the project itsself.
+•Added dumby data for testing
+•Created ability for user to push information to the DB</t>
+  </si>
+  <si>
+    <t>9:00am
+11:00am
+6:30pm</t>
+  </si>
+  <si>
+    <t>11:00am
+12:00am
+8:30pm</t>
+  </si>
+  <si>
+    <t>•Started creating my DB schema
+•Created DB schema</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
@@ -34,12 +102,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,8 +128,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,16 +423,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="77.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="88.77734375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>42639</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>42640</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>42641</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>42642</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>42643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>42644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>42645</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>42646</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>42647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>42648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>42649</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>42650</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>42651</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>42652</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>42653</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>42654</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>42655</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>42656</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>42657</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>42658</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>42659</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>42660</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>42661</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>42662</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>42664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>42665</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>42666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>42669</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>